<commit_message>
Auto Search implemented for DistCode Drop down
</commit_message>
<xml_diff>
--- a/Excel/Sample.xlsx
+++ b/Excel/Sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFB76E1-F7A2-4D6E-888D-C31AE0819C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F49CB2-961E-4AB5-9B91-C6FDD5D43284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distributor Info" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
   <si>
     <t>Distributor Master</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t xml:space="preserve">      The mandatory columns must not contain any blank or empty cells within the data. Please ensure all required fields are filled and try again.</t>
+  </si>
+  <si>
+    <t>POPULATION</t>
   </si>
 </sst>
 </file>
@@ -1056,6 +1059,18 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1070,18 +1085,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1403,11 +1406,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="15.5">
@@ -1475,7 +1478,7 @@
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="44" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1485,7 +1488,7 @@
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="41"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
@@ -1493,7 +1496,7 @@
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -1503,7 +1506,7 @@
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" ht="15.5">
-      <c r="A12" s="41"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
@@ -1681,10 +1684,10 @@
       <c r="A1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="38" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="23" t="s">
@@ -1699,22 +1702,22 @@
       <c r="G1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="37" t="s">
         <v>48</v>
       </c>
       <c r="I1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="37" t="s">
         <v>53</v>
       </c>
       <c r="N1" s="19" t="s">
@@ -5507,10 +5510,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5519,47 +5522,51 @@
     <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:11" ht="15.5">
+      <c r="A1" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="I1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="J1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="K1" s="39" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.5">
+    <row r="2" spans="1:11" ht="15.5">
       <c r="A2" s="20"/>
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
@@ -5570,8 +5577,9 @@
       <c r="H2" s="22"/>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.5">
+      <c r="K2" s="22"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.5">
       <c r="A3" s="20"/>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>
@@ -5582,8 +5590,9 @@
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.5">
+      <c r="K3" s="22"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.5">
       <c r="A4" s="20"/>
       <c r="B4" s="21"/>
       <c r="C4" s="22"/>
@@ -5594,8 +5603,9 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.5">
+      <c r="K4" s="22"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.5">
       <c r="A5" s="20"/>
       <c r="B5" s="21"/>
       <c r="C5" s="22"/>
@@ -5606,8 +5616,9 @@
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.5">
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.5">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
@@ -5618,6 +5629,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5628,7 +5640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AEBD87-F4F0-4306-8A40-6EE8CB604D11}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>

</xml_diff>